<commit_message>
Add line amp data
</commit_message>
<xml_diff>
--- a/model/outputData/Case_Runs.xlsx
+++ b/model/outputData/Case_Runs.xlsx
@@ -8,24 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex Palomino\Documents\GitHub\PGIA-Model\model\outputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE93C48F-BB4B-4343-A862-9C40182D6CF6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130C5ABE-1C5E-459C-A8EA-8558764F4D5A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50" yWindow="260" windowWidth="8690" windowHeight="5830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
   <si>
     <t>Base</t>
   </si>
@@ -440,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G14"/>
+  <dimension ref="B2:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,7 +541,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>10</v>
@@ -548,84 +553,86 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C10" s="5" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C11" s="2"/>
-      <c r="D11" s="6" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C10" s="2"/>
+      <c r="D10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="7"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>2</v>
+      <c r="B12" s="3">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B14" s="3">
-        <v>8</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="C2:G2"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
   </mergeCells>

</xml_diff>